<commit_message>
first commit for selenium java automation tests
</commit_message>
<xml_diff>
--- a/src/main/resources/saucedemotestdata.xlsx
+++ b/src/main/resources/saucedemotestdata.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>username</t>
   </si>
@@ -30,6 +30,24 @@
   </si>
   <si>
     <t>Epic sadface: Sorry, this user has been locked out.</t>
+  </si>
+  <si>
+    <t>locked</t>
+  </si>
+  <si>
+    <t>secret</t>
+  </si>
+  <si>
+    <t>Epic sadface: Username and password do not match any user in this service</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Epic sadface: Username is required</t>
+  </si>
+  <si>
+    <t>Epic sadface: Password is required</t>
   </si>
   <si>
     <t>productname</t>
@@ -60,6 +78,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -87,11 +108,17 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -314,7 +341,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.0"/>
+    <col customWidth="1" min="1" max="1" width="20.5"/>
+    <col customWidth="1" min="2" max="2" width="15.0"/>
+    <col customWidth="1" min="3" max="3" width="21.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -337,6 +366,39 @@
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -354,62 +416,62 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.5"/>
+    <col customWidth="1" min="1" max="1" width="21.38"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3">
         <v>29.99</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3">
         <v>15.99</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3">
         <v>7.99</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3">
         <v>9.99</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3">
         <v>49.99</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3">
         <v>15.99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new test in product
Added new test in product
moved files from main to test
</commit_message>
<xml_diff>
--- a/src/main/resources/saucedemotestdata.xlsx
+++ b/src/main/resources/saucedemotestdata.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>username</t>
   </si>
@@ -23,6 +23,18 @@
     <t>results</t>
   </si>
   <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Epic sadface: Username is required</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>Epic sadface: Password is required</t>
+  </si>
+  <si>
     <t>locked_out_user</t>
   </si>
   <si>
@@ -41,15 +53,6 @@
     <t>Epic sadface: Username and password do not match any user in this service</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>Epic sadface: Username is required</t>
-  </si>
-  <si>
-    <t>Epic sadface: Password is required</t>
-  </si>
-  <si>
     <t>productname</t>
   </si>
   <si>
@@ -71,7 +74,7 @@
     <t>Sauce Labs Fleece Jacket</t>
   </si>
   <si>
-    <t>T-Shirt Red</t>
+    <t>Test.allTheThings() T-Shirt (Red)</t>
   </si>
 </sst>
 </file>
@@ -108,14 +111,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -362,43 +362,43 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -421,57 +421,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2">
         <v>29.99</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="3">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2">
         <v>15.99</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="3">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2">
         <v>7.99</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="3">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2">
         <v>9.99</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="3">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2">
         <v>49.99</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="3">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2">
         <v>15.99</v>
       </c>
     </row>

</xml_diff>